<commit_message>
update: reservoir bounds changed to circle with const pressure
</commit_message>
<xml_diff>
--- a/data/constraint_settings.xlsx
+++ b/data/constraint_settings.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\79778\Desktop\streamlit_orchestrator\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\79778\Desktop\job\programmes\orchestrator\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{031D8DC7-307F-46B3-BCCA-713DC7488E48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D218F171-EB20-40C8-B45C-150282CE1F3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
-  <si>
-    <t>boundary_code</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>permeability</t>
   </si>
@@ -36,12 +33,6 @@
     <t>skin</t>
   </si>
   <si>
-    <t>res_width</t>
-  </si>
-  <si>
-    <t>res_length</t>
-  </si>
-  <si>
     <t>pressure_initial</t>
   </si>
   <si>
@@ -81,9 +72,6 @@
     <t>{"is_discrete": false, "bounds": [10, 300], "val_test_period": 100}</t>
   </si>
   <si>
-    <t>{"is_discrete": true, "bounds": [0, 1, 2, 3, 4, 5], "val_test_period": 0}</t>
-  </si>
-  <si>
     <t>{"is_discrete": true, "bounds": [2, 3, 4, 5, 6], "val_test_period": 5}</t>
   </si>
   <si>
@@ -100,6 +88,9 @@
   </si>
   <si>
     <t>{"is_discrete": false, "bounds": [40, 300], "val_test_period": 200}</t>
+  </si>
+  <si>
+    <t>res_radius</t>
   </si>
 </sst>
 </file>
@@ -417,35 +408,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="53" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="51.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="45.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="52.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="49.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="53.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="50.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="53" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="52.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="49.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="53.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="50.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="53" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -454,79 +444,67 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="B4" t="s">
         <v>18</v>
       </c>
-      <c r="C2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" t="s">
-        <v>24</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="G4" t="s">
         <v>14</v>
-      </c>
-      <c r="I2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>21</v>
-      </c>
-      <c r="I3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>22</v>
-      </c>
-      <c r="I4" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>